<commit_message>
EPBDS-10194 Revert test with comment.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10194_Casts.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10194_Casts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\SprArrTernaryCast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BF3E07-59A4-4381-8A5E-C0A256192A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2BABF2-29F5-4A1E-B8B4-F7941CA4A90D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="2170" windowWidth="22680" windowHeight="17060" xr2:uid="{1A980729-BA2F-495B-979A-9198E2B3CFD9}"/>
+    <workbookView xWindow="1520" yWindow="1100" windowWidth="22590" windowHeight="11780" xr2:uid="{1A980729-BA2F-495B-979A-9198E2B3CFD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Steps</t>
   </si>
@@ -84,15 +84,9 @@
     <t>= true ? new Integer[0] : "Hello"</t>
   </si>
   <si>
-    <t>Step5</t>
-  </si>
-  <si>
     <t>StepX</t>
   </si>
   <si>
-    <t>= sum($Step1.$StepX)</t>
-  </si>
-  <si>
     <t>Step6</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>_res_.$Step5</t>
-  </si>
-  <si>
     <t>_res_.$Step6</t>
   </si>
   <si>
@@ -132,7 +123,10 @@
     <t>1,2</t>
   </si>
   <si>
-    <t>java.io.Serializable</t>
+    <t>java.lang.Object</t>
+  </si>
+  <si>
+    <t>// true ? Policy[] : Double -&gt; should be Object (not Object[]). Please, don't do this</t>
   </si>
 </sst>
 </file>
@@ -176,12 +170,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -499,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6F2B0F-0684-44A3-B583-438B4F1D7539}">
-  <dimension ref="A2:N51"/>
+  <dimension ref="A2:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,7 +517,7 @@
     </row>
     <row r="4" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
@@ -545,7 +540,7 @@
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>3</v>
@@ -553,18 +548,18 @@
       <c r="L8" s="1"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D12" s="4" t="s">
@@ -592,37 +587,37 @@
       <c r="D13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C18" s="3"/>
@@ -725,7 +720,7 @@
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>21</v>
@@ -743,12 +738,8 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -762,7 +753,9 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -778,11 +771,17 @@
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -795,20 +794,18 @@
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -820,22 +817,22 @@
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="J29" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -844,21 +841,11 @@
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="3">
-        <v>5</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -883,17 +870,15 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
@@ -977,13 +962,13 @@
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -1013,9 +998,6 @@
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1023,7 +1005,6 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
-      <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D43" s="3"/>
@@ -1096,15 +1077,6 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.35">
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>